<commit_message>
fix: updating ROA xls
</commit_message>
<xml_diff>
--- a/static/files/DC_ROI_PAYBACK.xlsx
+++ b/static/files/DC_ROI_PAYBACK.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munja/git/datacontroller.io/static/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasdemo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE8451C-4F6A-ED4C-A8BB-54C922DB0A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="500" windowWidth="31180" windowHeight="20620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="225" yWindow="495" windowWidth="31185" windowHeight="20625"/>
   </bookViews>
   <sheets>
     <sheet name="Calculator" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
   <si>
     <t>1 - Development Time</t>
   </si>
@@ -99,9 +98,6 @@
     <t>Total Annual Savings</t>
   </si>
   <si>
-    <t>Number of Data Controller users</t>
-  </si>
-  <si>
     <t>Total Annual Cost</t>
   </si>
   <si>
@@ -138,9 +134,6 @@
     <t>Audits</t>
   </si>
   <si>
-    <t>Licences</t>
-  </si>
-  <si>
     <t>Months</t>
   </si>
   <si>
@@ -175,18 +168,21 @@
   </si>
   <si>
     <t>Aggregate average time saved per month</t>
+  </si>
+  <si>
+    <t>DC Licence / Support Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -701,61 +697,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" customWidth="1"/>
-    <col min="3" max="3" width="40.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="21">
       <c r="B2" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="23" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="23" t="s">
-        <v>31</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5">
       <c r="C6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D6" s="4">
         <v>550</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
       <c r="C7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D7" s="4">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
       <c r="C8" s="1" t="s">
         <v>1</v>
       </c>
@@ -764,37 +760,37 @@
         <v>33000</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
       <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5">
       <c r="C11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" s="4">
         <v>500</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12" s="4">
         <v>1.5</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
       <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
@@ -803,37 +799,37 @@
         <v>9000</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5">
       <c r="C16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="4">
         <v>500</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
       <c r="C17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D17" s="4">
         <v>1.5</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
       <c r="C18" s="1" t="s">
         <v>1</v>
       </c>
@@ -842,37 +838,37 @@
         <v>9000</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5">
       <c r="C21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21" s="4">
         <v>500</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
       <c r="C22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22" s="4">
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
       <c r="C23" s="1" t="s">
         <v>1</v>
       </c>
@@ -881,15 +877,15 @@
         <v>24000</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
       <c r="B25" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:5">
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
@@ -897,32 +893,32 @@
         <v>1000</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
       <c r="C27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D27" s="4">
         <v>2000</v>
       </c>
       <c r="E27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
       <c r="C28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D28" s="4">
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
       <c r="C29" t="s">
         <v>7</v>
       </c>
@@ -930,10 +926,10 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
       <c r="C30" s="1" t="s">
         <v>1</v>
       </c>
@@ -942,10 +938,10 @@
         <v>10000</v>
       </c>
       <c r="E30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
       <c r="C31" t="s">
         <v>8</v>
       </c>
@@ -953,7 +949,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:5">
       <c r="C32" t="s">
         <v>9</v>
       </c>
@@ -961,57 +957,57 @@
         <v>10000000</v>
       </c>
       <c r="E32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
       <c r="C33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D33" s="5">
         <v>0.25</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5">
       <c r="C34" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D34" s="1">
         <f>(D32*D31)*D33</f>
         <v>18750</v>
       </c>
       <c r="E34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
       <c r="B36" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5">
       <c r="C37" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D37" s="4">
         <v>500</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
       <c r="C38" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D38" s="4">
         <v>2</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5">
       <c r="C39" s="1" t="s">
         <v>1</v>
       </c>
@@ -1020,37 +1016,37 @@
         <v>12000</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
       <c r="B41" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5">
       <c r="C42" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D42" s="4">
         <v>500</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
       <c r="C43" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D43" s="4">
         <v>1</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5">
       <c r="C44" s="1" t="s">
         <v>1</v>
       </c>
@@ -1059,15 +1055,15 @@
         <v>6000</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5">
       <c r="B46" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5">
       <c r="B47" s="3"/>
       <c r="C47" t="s">
         <v>12</v>
@@ -1076,10 +1072,10 @@
         <v>1000</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5">
       <c r="B48" s="3"/>
       <c r="C48" t="s">
         <v>13</v>
@@ -1088,10 +1084,10 @@
         <v>2000</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5">
       <c r="B49" s="3"/>
       <c r="C49" t="s">
         <v>14</v>
@@ -1100,10 +1096,10 @@
         <v>1000</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5">
       <c r="B50" s="3"/>
       <c r="C50" t="s">
         <v>15</v>
@@ -1112,10 +1108,10 @@
         <v>4000</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5">
       <c r="B51" s="3"/>
       <c r="C51" t="s">
         <v>16</v>
@@ -1124,10 +1120,10 @@
         <v>2000</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5">
       <c r="B52" s="3"/>
       <c r="C52" t="s">
         <v>17</v>
@@ -1136,10 +1132,10 @@
         <v>1000</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5">
       <c r="B53" s="3"/>
       <c r="C53" t="s">
         <v>18</v>
@@ -1148,10 +1144,10 @@
         <v>1000</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5">
       <c r="B54" s="3"/>
       <c r="C54" t="s">
         <v>19</v>
@@ -1160,10 +1156,10 @@
         <v>1000</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5">
       <c r="B55" s="3"/>
       <c r="C55" t="s">
         <v>20</v>
@@ -1172,10 +1168,10 @@
         <v>1000</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5">
       <c r="B58" s="1" t="s">
         <v>21</v>
       </c>
@@ -1184,76 +1180,81 @@
         <v>136750</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5">
       <c r="C60" t="s">
+        <v>46</v>
+      </c>
+      <c r="D60">
+        <v>12000</v>
+      </c>
+      <c r="E60" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5">
+      <c r="B62" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D60">
-        <v>20</v>
-      </c>
-      <c r="E60" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B62" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="10">
-        <f>MIN(D60*500,100000)</f>
-        <v>10000</v>
+        <f>D60</f>
+        <v>12000</v>
       </c>
       <c r="E62" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" ht="21" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="21">
       <c r="B64" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C64" s="12"/>
       <c r="D64" s="20">
         <f>D58-D62</f>
-        <v>126750</v>
+        <v>124750</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" ht="21" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="21">
       <c r="B65" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C65" s="14"/>
       <c r="D65" s="21">
         <f>(D58-D62)/D62</f>
-        <v>12.675000000000001</v>
+        <v>10.395833333333334</v>
       </c>
       <c r="E65" s="18"/>
     </row>
-    <row r="66" spans="2:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" ht="21">
       <c r="B66" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C66" s="16"/>
       <c r="D66" s="22">
         <f>D62/D58*12</f>
-        <v>0.87751371115173682</v>
+        <v>1.0530164533820841</v>
       </c>
       <c r="E66" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:D3"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D60">
+      <formula1>"0,12000,25000"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{03A938A5-170E-364C-99ED-FBEFF088B21E}"/>
+    <hyperlink ref="B3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>